<commit_message>
update QT counts to HEWR only
</commit_message>
<xml_diff>
--- a/data/QT/Count_summary_QT.xlsx
+++ b/data/QT/Count_summary_QT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/QT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B304E3B-F716-9349-9D2D-FC667F119C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A87C813-5273-B542-A1AD-33A91B37B88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="500" windowWidth="29500" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Seip and Pelltier 2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimate was 129 in report, rounding difference </t>
-  </si>
-  <si>
     <t>MinCount_ADULTMF</t>
   </si>
   <si>
@@ -117,6 +114,18 @@
   </si>
   <si>
     <t>#'s from KMB updated gov #'s</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>HEWR</t>
+  </si>
+  <si>
+    <t>HEWR+rugged west</t>
+  </si>
+  <si>
+    <t>Estimate was 129 in report. Note (BM): We used the population estimate based strictly on the caribou seen within the survey area. // MC: This is the estimate for the entire population when we correct for 24% of the population that may have been outside the census area (i.e. four of the 17 radio-collared caribou were outside the census area.). Note (BM): Another MC population estimate is given; 129 caribou, with a lower and upper 95% CI of (114, 129) and a SCF of 0.76. "This is the estimate for the entire population when we correct for 24% of the population that may have been outside the census area (i.e. four of the 17 radio-collared caribou were outside the census area.)" // Note (BM): Confidence level for population estimate is 95%.</t>
   </si>
 </sst>
 </file>
@@ -972,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,7 +1003,7 @@
     <col min="16" max="16" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,13 +1011,13 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -1038,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
         <v>1</v>
@@ -1049,8 +1058,11 @@
       <c r="R1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2001</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -1118,8 +1130,11 @@
       <c r="R3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2003</v>
       </c>
@@ -1127,7 +1142,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -1136,7 +1151,7 @@
       </c>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2005</v>
       </c>
@@ -1144,7 +1159,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2006</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2007</v>
       </c>
@@ -1160,7 +1175,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -1216,8 +1231,11 @@
       <c r="P9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2009</v>
       </c>
@@ -1225,7 +1243,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -1233,7 +1251,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -1241,7 +1259,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2012</v>
       </c>
@@ -1249,7 +1267,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2013</v>
       </c>
@@ -1259,13 +1277,13 @@
       </c>
       <c r="C14">
         <f>SUM(D14:E14)</f>
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="D14">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>78</v>
@@ -1306,10 +1324,13 @@
         <v>12</v>
       </c>
       <c r="Q14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="S14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2014</v>
       </c>
@@ -1317,7 +1338,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2015</v>
       </c>
@@ -1335,13 +1356,13 @@
       </c>
       <c r="C17">
         <f>SUM(D17:E17)</f>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D17">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <v>22</v>
@@ -1382,7 +1403,7 @@
         <v>18</v>
       </c>
       <c r="Q17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -1450,7 +1471,7 @@
         <v>19</v>
       </c>
       <c r="Q19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -1510,7 +1531,7 @@
         <v>20</v>
       </c>
       <c r="Q20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -1576,7 +1597,7 @@
         <v>120.75471698113206</v>
       </c>
       <c r="P22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>